<commit_message>
First try at catch MSY
</commit_message>
<xml_diff>
--- a/raw_data/finalfocalspecies.xlsx
+++ b/raw_data/finalfocalspecies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selen\Google Drive\UCSB_MSc\MidriffsWatch\GitHub\2019GP\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selen\Documents\GitHub\2019GP\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189F18A3-BF2F-42C1-BFBF-A6EADBFF4705}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBB0B4D-DB31-45FC-9D20-0D10F76C67F1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" xr2:uid="{37877605-6F1C-4C9B-BB9B-3C6C61EA15C4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="66">
   <si>
     <t>CommonName</t>
   </si>
@@ -223,72 +223,6 @@
   </si>
   <si>
     <t>Abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Habitat </t>
-  </si>
-  <si>
-    <t>reef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth </t>
-  </si>
-  <si>
-    <t>Max_length_cm</t>
-  </si>
-  <si>
-    <t>Common_length_cm</t>
-  </si>
-  <si>
-    <t>Max_published_weight_kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 to 30 </t>
-  </si>
-  <si>
-    <t>IUCN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Least concern </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 to 60 </t>
-  </si>
-  <si>
-    <t>3 to 80</t>
-  </si>
-  <si>
-    <t>50 to X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demersal </t>
-  </si>
-  <si>
-    <t>30 to X</t>
-  </si>
-  <si>
-    <t>3 to 40</t>
-  </si>
-  <si>
-    <t>10 to 60</t>
-  </si>
-  <si>
-    <t>reed</t>
-  </si>
-  <si>
-    <t>8 to 55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near threatened </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endangered </t>
-  </si>
-  <si>
-    <t>5 to 30</t>
-  </si>
-  <si>
-    <t>rocky reef</t>
   </si>
 </sst>
 </file>
@@ -324,9 +258,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,13 +574,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DCC5AE-8DD8-407D-80D8-85413909590A}">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,17 +588,13 @@
     <col min="1" max="1" width="15.6328125" customWidth="1"/>
     <col min="2" max="2" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" customWidth="1"/>
     <col min="16" max="16" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.81640625" customWidth="1"/>
-    <col min="19" max="19" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -720,26 +649,8 @@
       <c r="R1" t="s">
         <v>64</v>
       </c>
-      <c r="S1" t="s">
-        <v>66</v>
-      </c>
-      <c r="T1" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -794,26 +705,8 @@
       <c r="R2" t="s">
         <v>62</v>
       </c>
-      <c r="S2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U2">
-        <v>51</v>
-      </c>
-      <c r="V2">
-        <v>30</v>
-      </c>
-      <c r="W2">
-        <v>3.6</v>
-      </c>
-      <c r="X2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -868,23 +761,8 @@
       <c r="R3" t="s">
         <v>62</v>
       </c>
-      <c r="S3" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="U3">
-        <v>76</v>
-      </c>
-      <c r="V3">
-        <v>50</v>
-      </c>
-      <c r="X3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -939,23 +817,8 @@
       <c r="R4" t="s">
         <v>62</v>
       </c>
-      <c r="S4" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="U4">
-        <v>61</v>
-      </c>
-      <c r="W4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="X4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1010,23 +873,8 @@
       <c r="R5" t="s">
         <v>62</v>
       </c>
-      <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="U5">
-        <v>114</v>
-      </c>
-      <c r="W5">
-        <v>22.3</v>
-      </c>
-      <c r="X5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1081,20 +929,8 @@
       <c r="R6" t="s">
         <v>62</v>
       </c>
-      <c r="S6" t="s">
-        <v>78</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="U6">
-        <v>60</v>
-      </c>
-      <c r="X6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1149,21 +985,8 @@
       <c r="R7" t="s">
         <v>62</v>
       </c>
-      <c r="S7" t="s">
-        <v>78</v>
-      </c>
-      <c r="T7" s="1"/>
-      <c r="U7">
-        <v>42</v>
-      </c>
-      <c r="V7">
-        <v>35</v>
-      </c>
-      <c r="X7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1212,23 +1035,8 @@
       <c r="P8" t="s">
         <v>55</v>
       </c>
-      <c r="S8" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U8">
-        <v>35</v>
-      </c>
-      <c r="V8">
-        <v>30</v>
-      </c>
-      <c r="X8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1283,23 +1091,8 @@
       <c r="R9" t="s">
         <v>62</v>
       </c>
-      <c r="S9" t="s">
-        <v>67</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="U9">
-        <v>71</v>
-      </c>
-      <c r="W9">
-        <v>13</v>
-      </c>
-      <c r="X9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1354,23 +1147,8 @@
       <c r="R10" t="s">
         <v>62</v>
       </c>
-      <c r="S10" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="U10">
-        <v>80</v>
-      </c>
-      <c r="W10">
-        <v>1.3</v>
-      </c>
-      <c r="X10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1425,23 +1203,8 @@
       <c r="R11" t="s">
         <v>62</v>
       </c>
-      <c r="S11" t="s">
-        <v>82</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U11">
-        <v>198</v>
-      </c>
-      <c r="W11">
-        <v>91</v>
-      </c>
-      <c r="X11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1493,23 +1256,8 @@
       <c r="Q12" t="s">
         <v>62</v>
       </c>
-      <c r="S12" t="s">
-        <v>67</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="U12">
-        <v>105</v>
-      </c>
-      <c r="W12">
-        <v>14.1</v>
-      </c>
-      <c r="X12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1561,21 +1309,8 @@
       <c r="Q13" t="s">
         <v>62</v>
       </c>
-      <c r="S13" t="s">
-        <v>87</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="U13">
-        <v>38</v>
-      </c>
-      <c r="V13">
-        <v>30</v>
-      </c>
-      <c r="X13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1627,20 +1362,8 @@
       <c r="Q14" t="s">
         <v>62</v>
       </c>
-      <c r="S14" t="s">
-        <v>87</v>
-      </c>
-      <c r="T14" s="1">
-        <v>65</v>
-      </c>
-      <c r="U14">
-        <v>90</v>
-      </c>
-      <c r="V14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1695,9 +1418,8 @@
       <c r="R15" t="s">
         <v>63</v>
       </c>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1752,9 +1474,8 @@
       <c r="R16" t="s">
         <v>62</v>
       </c>
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1794,9 +1515,8 @@
       <c r="P17" t="s">
         <v>55</v>
       </c>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1842,10 +1562,6 @@
       <c r="R18" t="s">
         <v>63</v>
       </c>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="T19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Filtered using landing sites in MRI and updated MSY_Trial rmd.
</commit_message>
<xml_diff>
--- a/raw_data/finalfocalspecies.xlsx
+++ b/raw_data/finalfocalspecies.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selen\Documents\GitHub\2019GP\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9763F26-409E-4871-B4D9-CECD99001FF1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD41B0FA-DBE8-4A7C-B720-45512967248F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" xr2:uid="{37877605-6F1C-4C9B-BB9B-3C6C61EA15C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="94">
   <si>
     <t>CommonName</t>
   </si>
@@ -255,12 +256,84 @@
   <si>
     <t>Octopus sp</t>
   </si>
+  <si>
+    <t>Cynocsion sp</t>
+  </si>
+  <si>
+    <t>Cynoscion arenarius</t>
+  </si>
+  <si>
+    <t>Cynoscion nothus</t>
+  </si>
+  <si>
+    <t>Cynoscion othonopterus</t>
+  </si>
+  <si>
+    <t>Cynoscion parvipinnis</t>
+  </si>
+  <si>
+    <t>Cynoscion reticulatus</t>
+  </si>
+  <si>
+    <t>Cynoscion xanthulus</t>
+  </si>
+  <si>
+    <t>Dosidicus gigas</t>
+  </si>
+  <si>
+    <t>Etrumeus teres</t>
+  </si>
+  <si>
+    <t>Farfantepenaeus californiensis</t>
+  </si>
+  <si>
+    <t>Farfantepenaeus duorarum</t>
+  </si>
+  <si>
+    <t>Información no disponible</t>
+  </si>
+  <si>
+    <t>Litopenaeus stylirostris</t>
+  </si>
+  <si>
+    <t>Loligo vulgaris</t>
+  </si>
+  <si>
+    <t>Loliolopsis diomedeae</t>
+  </si>
+  <si>
+    <t>N/d</t>
+  </si>
+  <si>
+    <t>NANA</t>
+  </si>
+  <si>
+    <t>No disponible</t>
+  </si>
+  <si>
+    <t>Penaeus sp</t>
+  </si>
+  <si>
+    <t>Penaeus spp</t>
+  </si>
+  <si>
+    <t>Sicyonia penicillata</t>
+  </si>
+  <si>
+    <t>Trachypenaeus faoe</t>
+  </si>
+  <si>
+    <t>Trachypenaeus pacificus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,16 +347,65 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0F0F0F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4E5C68"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -291,15 +413,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0C1F30"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,13 +774,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DCC5AE-8DD8-407D-80D8-85413909590A}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="R22" sqref="R22:S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -629,9 +792,10 @@
     <col min="16" max="16" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.81640625" customWidth="1"/>
+    <col min="20" max="20" width="12" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -689,120 +853,129 @@
       <c r="S1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="T1" s="11">
+        <v>76591.820000000007</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="9">
+        <v>2.250683E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>12</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>12</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>25</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>22.5</v>
       </c>
-      <c r="N3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="N3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" t="s">
-        <v>62</v>
-      </c>
-      <c r="R3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="9">
+        <v>5.1971109999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -857,8 +1030,9 @@
       <c r="R4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -913,8 +1087,9 @@
       <c r="R5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -969,8 +1144,9 @@
       <c r="R6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1025,8 +1201,9 @@
       <c r="R7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1075,64 +1252,68 @@
       <c r="P8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>35</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>45</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>40</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>45</v>
       </c>
-      <c r="L9">
-        <v>50</v>
-      </c>
-      <c r="M9">
+      <c r="L9" s="1">
+        <v>50</v>
+      </c>
+      <c r="M9" s="1">
         <v>47.5</v>
       </c>
-      <c r="N9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" t="s">
-        <v>51</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="N9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q9" t="s">
-        <v>62</v>
-      </c>
-      <c r="R9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T9" s="9">
+        <v>4.1841480000000001E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1187,67 +1368,71 @@
       <c r="R10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="T10" s="8"/>
+    </row>
+    <row r="11" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G11">
-        <v>50</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="1">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1">
         <v>60</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>55</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K11">
-        <v>50</v>
-      </c>
-      <c r="L11">
+      <c r="K11" s="1">
+        <v>50</v>
+      </c>
+      <c r="L11" s="1">
         <v>60</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>55</v>
       </c>
-      <c r="N11" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" t="s">
-        <v>51</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="N11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q11" t="s">
-        <v>62</v>
-      </c>
-      <c r="R11" t="s">
-        <v>62</v>
-      </c>
-      <c r="S11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T11" s="9">
+        <v>3.7158969999999999E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1299,8 +1484,9 @@
       <c r="Q12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1355,8 +1541,9 @@
       <c r="S13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T13" s="8"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1408,8 +1595,9 @@
       <c r="Q14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1467,8 +1655,9 @@
       <c r="S15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1526,8 +1715,9 @@
       <c r="S16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T16" s="8"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1567,55 +1757,59 @@
       <c r="P17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="T17" s="8"/>
+    </row>
+    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>30</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>30</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>30</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N18" t="s">
-        <v>51</v>
-      </c>
-      <c r="O18" t="s">
-        <v>51</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="N18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q18" t="s">
-        <v>62</v>
-      </c>
-      <c r="R18" t="s">
+      <c r="Q18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T18" s="10">
+        <v>9.1491670000000002E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1664,55 +1858,413 @@
       <c r="S19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="T19" s="8"/>
+    </row>
+    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>40</v>
       </c>
-      <c r="H20">
-        <v>50</v>
-      </c>
-      <c r="I20">
+      <c r="H20" s="1">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1">
         <v>45</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="1">
         <v>100</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>120</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="1">
         <v>110</v>
       </c>
-      <c r="Q20" t="s">
-        <v>50</v>
-      </c>
-      <c r="R20" t="s">
-        <v>51</v>
-      </c>
-      <c r="S20" t="s">
-        <v>50</v>
+      <c r="Q20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T20" s="10">
+        <v>1.4733E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="R22" s="7">
+        <v>0.29277809999999999</v>
+      </c>
+      <c r="S22" s="7">
+        <v>0.11348750000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECAAA46-7F43-4EDF-81AF-B109F329D799}">
+  <dimension ref="A2:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4">
+        <v>184.56032999999999</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.4991289999999999E-2</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.19</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.611378E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="4">
+        <v>16.940069999999999</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2.2938530000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="4">
+        <v>71.888769999999994</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9.7344519999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.36764E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8.3954139999999999E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2.9248540000000002E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="6">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4438.8865800000003</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.60106919999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="6">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="4">
+        <v>27.880600000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3.7753090000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="4">
+        <v>16.89507</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2.2877589999999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="6">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.4470000000000001</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3.3134800000000003E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="6">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1942.00218</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.26296629999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="6">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="4">
+        <v>153.88831999999999</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2.0837999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="6">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4">
+        <v>22.86</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3.0954699999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="4">
+        <v>31.30641</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4.2391970000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="6">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="6">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="4">
+        <v>296.06939999999997</v>
+      </c>
+      <c r="D20" s="5">
+        <v>4.0090729999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="6">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="4">
+        <v>104.95198000000001</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.421154E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="6">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="4">
+        <v>52.816949999999999</v>
+      </c>
+      <c r="D22" s="5">
+        <v>7.151938E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="6">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="4">
+        <v>10</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1.3540990000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="6">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="4">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D24" s="5">
+        <v>6.0663630000000002E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="6">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="4">
+        <v>3.04</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4.1164609999999998E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>